<commit_message>
19th September 2017, 06:33 PM
</commit_message>
<xml_diff>
--- a/POM/keywords/TC001.xlsx
+++ b/POM/keywords/TC001.xlsx
@@ -10,7 +10,6 @@
     <sheet name="TC001" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -44,9 +43,6 @@
     <t>/html/body/div[20]/div/div[2]/div[2]/div[2]/form/div[2]/input</t>
   </si>
   <si>
-    <t>rohith270419909940096410abcd1990</t>
-  </si>
-  <si>
     <t>/html/body/div[20]/div/div[2]/div[2]/div[2]/form/input[1]</t>
   </si>
   <si>
@@ -54,6 +50,9 @@
   </si>
   <si>
     <t>/html/body/div[2]/div[1]/div[2]/div/div/div[3]/ul/li[1]/div/ul/li[13]/button</t>
+  </si>
+  <si>
+    <t>rohith</t>
   </si>
 </sst>
 </file>
@@ -459,7 +458,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -526,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -534,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -543,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -552,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2"/>
     </row>

</xml_diff>